<commit_message>
Add cost model for adverse events
</commit_message>
<xml_diff>
--- a/data-raw/costs_ae.xlsx
+++ b/data-raw/costs_ae.xlsx
@@ -75,9 +75,6 @@
     <t>ast</t>
   </si>
   <si>
-    <t>eye_prob</t>
-  </si>
-  <si>
     <t>paronychia</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>ae_abb</t>
+  </si>
+  <si>
+    <t>eye_problems</t>
   </si>
 </sst>
 </file>
@@ -520,20 +520,21 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -548,7 +549,7 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -574,7 +575,7 @@
         <v>659.39987172942278</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -651,7 +652,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -674,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1">
         <v>7788</v>
@@ -692,7 +693,7 @@
         <v>794.70848050584118</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -700,7 +701,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1">
         <v>7728</v>
@@ -718,7 +719,7 @@
         <v>788.58591902274532</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -726,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -749,7 +750,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>7429</v>
@@ -772,7 +773,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1">
         <v>8101</v>
@@ -790,7 +791,7 @@
         <v>826.64784290932425</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update computation of adverse event costs
</commit_message>
<xml_diff>
--- a/data-raw/costs_ae.xlsx
+++ b/data-raw/costs_ae.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="costs_ae" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>mean</t>
   </si>
@@ -93,9 +93,6 @@
     <t>ref</t>
   </si>
   <si>
-    <t>DRG 808</t>
-  </si>
-  <si>
     <t>DRG 157</t>
   </si>
   <si>
@@ -112,6 +109,24 @@
   </si>
   <si>
     <t>eye_problems</t>
+  </si>
+  <si>
+    <t>Wong, William, et al. "Assessment of costs associated with adverse events in patients with cancer." PloS one 13.4 (2018): e0196007.</t>
+  </si>
+  <si>
+    <t>Used the cost estimate for dermatitis</t>
+  </si>
+  <si>
+    <t>Latremouille-Viau, Dominick, et al. "The economic burden of common adverse events associated with metastatic colorectal cancer treatment in the United States." Journal of medical economics 20.1 (2017): 54-62.</t>
+  </si>
+  <si>
+    <t>Used the adjusted monthly cost difference b/w individuals with hepatobiliary/pancreatic AEs and those without and multiplied by 12 for yearly estimate</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>DRG 391</t>
   </si>
 </sst>
 </file>
@@ -173,9 +188,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -517,24 +540,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.1640625" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -551,8 +576,11 @@
       <c r="G1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -574,11 +602,12 @@
         <f>(E2-D2)/(2*NORMSINV(0.975))</f>
         <v>659.39987172942278</v>
       </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -586,91 +615,113 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>940</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>752</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E11" si="1">C3*1.2</f>
-        <v>0</v>
+        <v>1128</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F11" si="2">(E3-D3)/(2*NORMSINV(0.975))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>95.920129901834969</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="3">
+        <v>3900</v>
+      </c>
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
+        <v>3120</v>
+      </c>
+      <c r="E4" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F4">
+        <v>4680</v>
+      </c>
+      <c r="F4" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>397.96649640123019</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="3">
+        <v>3900</v>
+      </c>
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
+        <v>3120</v>
+      </c>
+      <c r="E5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F5">
+        <v>4680</v>
+      </c>
+      <c r="F5" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>397.96649640123019</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2737</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2189.6</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3284.4</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>279.29084632055566</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -692,11 +743,12 @@
         <f t="shared" si="2"/>
         <v>794.70848050584118</v>
       </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -718,34 +770,39 @@
         <f t="shared" si="2"/>
         <v>788.58591902274532</v>
       </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="45">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" s="1">
+        <v>1184</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>947.2</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1420.8</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>120.81854659975806</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -753,22 +810,26 @@
         <v>21</v>
       </c>
       <c r="C10" s="1">
-        <v>7429</v>
+        <v>940</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>5943.2000000000007</v>
+        <v>752</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="1"/>
-        <v>8914.7999999999993</v>
+        <v>1128</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>758.07515429865066</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>95.920129901834969</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -790,9 +851,13 @@
         <f t="shared" si="2"/>
         <v>826.64784290932425</v>
       </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update non NMA parameter estimates
</commit_message>
<xml_diff>
--- a/data-raw/costs_ae.xlsx
+++ b/data-raw/costs_ae.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="costs_ae" sheetId="1" r:id="rId1"/>
@@ -111,15 +111,9 @@
     <t>eye_problems</t>
   </si>
   <si>
-    <t>Wong, William, et al. "Assessment of costs associated with adverse events in patients with cancer." PloS one 13.4 (2018): e0196007.</t>
-  </si>
-  <si>
     <t>Used the cost estimate for dermatitis</t>
   </si>
   <si>
-    <t>Latremouille-Viau, Dominick, et al. "The economic burden of common adverse events associated with metastatic colorectal cancer treatment in the United States." Journal of medical economics 20.1 (2017): 54-62.</t>
-  </si>
-  <si>
     <t>Used the adjusted monthly cost difference b/w individuals with hepatobiliary/pancreatic AEs and those without and multiplied by 12 for yearly estimate</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>DRG 391</t>
+  </si>
+  <si>
+    <t>wong2018assessment</t>
+  </si>
+  <si>
+    <t>latremouille2017economic</t>
   </si>
 </sst>
 </file>
@@ -175,8 +175,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -200,17 +206,23 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -577,7 +589,7 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -603,11 +615,11 @@
         <v>659.39987172942278</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="45">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -630,13 +642,13 @@
         <v>95.920129901834969</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="75">
+    </row>
+    <row r="4" spans="1:8" ht="60">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -659,13 +671,13 @@
         <v>397.96649640123019</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -688,13 +700,13 @@
         <v>397.96649640123019</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -717,7 +729,7 @@
         <v>279.29084632055566</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -775,7 +787,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="45">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -798,11 +810,11 @@
         <v>120.81854659975806</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="45">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -825,7 +837,7 @@
         <v>95.920129901834969</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H10" s="2"/>
     </row>

</xml_diff>

<commit_message>
AE costs and inpatient costs
</commit_message>
<xml_diff>
--- a/data-raw/costs_ae.xlsx
+++ b/data-raw/costs_ae.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/IVI/GitHub/IVI-NSCLC/data-raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F952ABF0-130E-A641-9869-657EB14F0FC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="10600" yWindow="5760" windowWidth="18500" windowHeight="13020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_ae" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>mean</t>
   </si>
@@ -99,9 +105,6 @@
     <t>DRG 602</t>
   </si>
   <si>
-    <t>DRG 193</t>
-  </si>
-  <si>
     <t>ae_name</t>
   </si>
   <si>
@@ -111,28 +114,25 @@
     <t>eye_problems</t>
   </si>
   <si>
-    <t>Used the cost estimate for dermatitis</t>
-  </si>
-  <si>
-    <t>Used the adjusted monthly cost difference b/w individuals with hepatobiliary/pancreatic AEs and those without and multiplied by 12 for yearly estimate</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>DRG 391</t>
-  </si>
-  <si>
     <t>wong2018assessment</t>
   </si>
   <si>
-    <t>latremouille2017economic</t>
+    <t>PinarBilir2016economic</t>
+  </si>
+  <si>
+    <t>Used the cost estimate for dermatitis all AE</t>
+  </si>
+  <si>
+    <t>Grade 3/4 from trials, severe AE (i.e. inpatient) assumed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -158,12 +158,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -201,10 +207,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -227,6 +233,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -551,14 +565,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -566,12 +580,12 @@
     <col min="8" max="8" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -589,10 +603,10 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -600,26 +614,26 @@
         <v>14</v>
       </c>
       <c r="C2" s="1">
-        <v>6462</v>
+        <v>16510</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D11" si="0">C2*0.8</f>
-        <v>5169.6000000000004</v>
+        <v>14090</v>
       </c>
       <c r="E2" s="1">
-        <f>C2*1.2</f>
-        <v>7754.4</v>
+        <v>18791</v>
       </c>
       <c r="F2">
-        <f>(E2-D2)/(2*NORMSINV(0.975))</f>
-        <v>659.39987172942278</v>
+        <f>(E2-D2)/3.92</f>
+        <v>1199.2346938775511</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -630,25 +644,23 @@
         <v>940</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" si="0"/>
-        <v>752</v>
+        <v>106</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E11" si="1">C3*1.2</f>
-        <v>1128</v>
+        <v>1844</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="2">(E3-D3)/(2*NORMSINV(0.975))</f>
-        <v>95.920129901834969</v>
+        <f>(E3-D3)/3.92</f>
+        <v>443.36734693877554</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="60">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -656,28 +668,28 @@
         <v>16</v>
       </c>
       <c r="C4" s="3">
-        <v>3900</v>
+        <v>19122</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="0"/>
-        <v>3120</v>
+        <f>C4-1.96*F4</f>
+        <v>7915.7615769072636</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="1"/>
-        <v>4680</v>
-      </c>
-      <c r="F4" s="4">
-        <f t="shared" si="2"/>
-        <v>397.96649640123019</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>35</v>
+        <f>C4+1.96*F4</f>
+        <v>30328.238423092735</v>
+      </c>
+      <c r="F4">
+        <f>15127/SQRT(7)</f>
+        <v>5717.4685832105797</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -685,55 +697,55 @@
         <v>17</v>
       </c>
       <c r="C5" s="3">
-        <v>3900</v>
+        <v>19122</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>3120</v>
+        <f>C5-1.96*F5</f>
+        <v>7915.7615769072636</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="1"/>
-        <v>4680</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" si="2"/>
-        <v>397.96649640123019</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>35</v>
+        <f>C5+1.96*F5</f>
+        <v>30328.238423092735</v>
+      </c>
+      <c r="F5">
+        <f>15127/SQRT(7)</f>
+        <v>5717.4685832105797</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1">
-        <v>2737</v>
+        <v>31975</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>2189.6</v>
+        <v>21923</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
-        <v>3284.4</v>
+        <v>49448</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
-        <v>279.29084632055566</v>
+        <f>(E6-D6)/3.92</f>
+        <v>7021.6836734693879</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -744,23 +756,23 @@
         <v>7788</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D2:D11" si="0">C7*0.8</f>
         <v>6230.4000000000005</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E3:E11" si="1">C7*1.2</f>
         <v>9345.6</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
-        <v>794.70848050584118</v>
+        <f>(E7-D7)/3.92</f>
+        <v>794.69387755102036</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -768,26 +780,26 @@
         <v>19</v>
       </c>
       <c r="C8" s="1">
-        <v>7728</v>
+        <v>21929</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>6182.4000000000005</v>
+        <v>20697</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>9273.6</v>
+        <v>23425</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
-        <v>788.58591902274532</v>
+        <f>(E8-D8)/3.92</f>
+        <v>695.91836734693879</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -795,53 +807,53 @@
         <v>20</v>
       </c>
       <c r="C9" s="1">
-        <v>1184</v>
+        <v>26172</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>947.2</v>
+        <v>3663</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
-        <v>1420.8</v>
+        <v>62005</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
-        <v>120.81854659975806</v>
+        <f>(E9-D9)/3.92</f>
+        <v>14883.163265306122</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1">
-        <v>940</v>
+      <c r="C10" s="5">
+        <v>15709</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>752</v>
+        <v>11315</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
-        <v>1128</v>
+        <v>21373</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>95.920129901834969</v>
+        <f>(E10-D10)/3.92</f>
+        <v>2565.8163265306125</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -860,15 +872,15 @@
         <v>9721.1999999999989</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
-        <v>826.64784290932425</v>
+        <f>(E11-D11)/3.92</f>
+        <v>826.63265306122423</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update parametr estimates, including in LaTeX documentation
</commit_message>
<xml_diff>
--- a/data-raw/costs_ae.xlsx
+++ b/data-raw/costs_ae.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/IVI/GitHub/IVI-NSCLC/data-raw/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F952ABF0-130E-A641-9869-657EB14F0FC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="5760" windowWidth="18500" windowHeight="13020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="costs_ae" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -120,19 +114,19 @@
     <t>wong2018assessment</t>
   </si>
   <si>
-    <t>PinarBilir2016economic</t>
-  </si>
-  <si>
     <t>Used the cost estimate for dermatitis all AE</t>
   </si>
   <si>
     <t>Grade 3/4 from trials, severe AE (i.e. inpatient) assumed</t>
+  </si>
+  <si>
+    <t>bilir2016economic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -565,14 +559,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -580,7 +574,7 @@
     <col min="8" max="8" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -606,7 +600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="34">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -630,10 +624,10 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -657,10 +651,10 @@
         <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -683,13 +677,13 @@
         <v>5717.4685832105797</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -712,13 +706,13 @@
         <v>5717.4685832105797</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="34">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -735,17 +729,17 @@
         <v>49448</v>
       </c>
       <c r="F6">
-        <f>(E6-D6)/3.92</f>
+        <f t="shared" ref="F6:F11" si="0">(E6-D6)/3.92</f>
         <v>7021.6836734693879</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -756,15 +750,15 @@
         <v>7788</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" ref="D2:D11" si="0">C7*0.8</f>
+        <f t="shared" ref="D7:D11" si="1">C7*0.8</f>
         <v>6230.4000000000005</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ref="E3:E11" si="1">C7*1.2</f>
+        <f t="shared" ref="E7:E11" si="2">C7*1.2</f>
         <v>9345.6</v>
       </c>
       <c r="F7">
-        <f>(E7-D7)/3.92</f>
+        <f t="shared" si="0"/>
         <v>794.69387755102036</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -772,7 +766,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="34">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -789,17 +783,17 @@
         <v>23425</v>
       </c>
       <c r="F8">
-        <f>(E8-D8)/3.92</f>
+        <f t="shared" si="0"/>
         <v>695.91836734693879</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -816,17 +810,17 @@
         <v>62005</v>
       </c>
       <c r="F9">
-        <f>(E9-D9)/3.92</f>
+        <f t="shared" si="0"/>
         <v>14883.163265306122</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="34">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -843,17 +837,17 @@
         <v>21373</v>
       </c>
       <c r="F10">
-        <f>(E10-D10)/3.92</f>
+        <f t="shared" si="0"/>
         <v>2565.8163265306125</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -864,15 +858,15 @@
         <v>8101</v>
       </c>
       <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>6480.8</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>9721.1999999999989</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="0"/>
-        <v>6480.8</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="1"/>
-        <v>9721.1999999999989</v>
-      </c>
-      <c r="F11">
-        <f>(E11-D11)/3.92</f>
         <v>826.63265306122423</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -880,7 +874,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="C14" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add adverse events to PDF documentation
</commit_message>
<xml_diff>
--- a/data-raw/costs_ae.xlsx
+++ b/data-raw/costs_ae.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="costs_ae" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>mean</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>ref</t>
-  </si>
-  <si>
-    <t>DRG 157</t>
   </si>
   <si>
     <t>DRG 602</t>
@@ -133,6 +130,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -152,18 +150,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -175,7 +167,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -193,8 +185,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -204,9 +200,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -215,6 +210,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -223,6 +220,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,7 +562,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -576,10 +575,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -597,10 +596,10 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="34">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -621,13 +620,13 @@
         <v>1199.2346938775511</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -648,10 +647,10 @@
         <v>443.36734693877554</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
@@ -677,10 +676,10 @@
         <v>5717.4685832105797</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
@@ -706,18 +705,18 @@
         <v>5717.4685832105797</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="34">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1">
         <v>31975</v>
@@ -733,13 +732,13 @@
         <v>7021.6836734693879</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -762,11 +761,11 @@
         <v>794.69387755102036</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="34">
+    <row r="8" spans="1:8" ht="30">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -787,13 +786,13 @@
         <v>695.91836734693879</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="34">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -814,20 +813,20 @@
         <v>14883.163265306122</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="34">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>15709</v>
       </c>
       <c r="D10" s="1">
@@ -841,13 +840,13 @@
         <v>2565.8163265306125</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -855,24 +854,24 @@
         <v>22</v>
       </c>
       <c r="C11" s="1">
-        <v>8101</v>
+        <v>18151</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
-        <v>6480.8</v>
+        <v>15111</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="2"/>
-        <v>9721.1999999999989</v>
+        <v>22542</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>826.63265306122423</v>
+        <v>1895.6632653061224</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="C14" s="1"/>

</xml_diff>

<commit_message>
Use medical CPI to inflate AE costs
</commit_message>
<xml_diff>
--- a/data-raw/costs_ae.xlsx
+++ b/data-raw/costs_ae.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>mean</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>bilir2016economic</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -189,8 +192,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -200,8 +205,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -212,6 +218,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -222,6 +229,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,21 +567,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.1640625" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.1640625" customWidth="1"/>
+    <col min="9" max="9" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -592,14 +601,17 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -619,14 +631,17 @@
         <f>(E2-D2)/3.92</f>
         <v>1199.2346938775511</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5">
+        <v>2015</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -646,14 +661,17 @@
         <f>(E3-D3)/3.92</f>
         <v>443.36734693877554</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5">
+        <v>2015</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -675,14 +693,17 @@
         <f>15127/SQRT(7)</f>
         <v>5717.4685832105797</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5">
+        <v>2014</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -704,14 +725,17 @@
         <f>15127/SQRT(7)</f>
         <v>5717.4685832105797</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5">
+        <v>2014</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -731,14 +755,17 @@
         <f t="shared" ref="F6:F11" si="0">(E6-D6)/3.92</f>
         <v>7021.6836734693879</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="5">
+        <v>2015</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -749,23 +776,26 @@
         <v>7788</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" ref="D7:D11" si="1">C7*0.8</f>
+        <f t="shared" ref="D7" si="1">C7*0.8</f>
         <v>6230.4000000000005</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ref="E7:E11" si="2">C7*1.2</f>
+        <f t="shared" ref="E7" si="2">C7*1.2</f>
         <v>9345.6</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>794.69387755102036</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="5">
+        <v>2016</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="30">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -785,14 +815,17 @@
         <f t="shared" si="0"/>
         <v>695.91836734693879</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="5">
+        <v>2015</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -812,14 +845,17 @@
         <f t="shared" si="0"/>
         <v>14883.163265306122</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="5">
+        <v>2015</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30">
+    <row r="10" spans="1:9" ht="30">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -839,14 +875,17 @@
         <f t="shared" si="0"/>
         <v>2565.8163265306125</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="5">
+        <v>2015</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:9" ht="30">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -866,14 +905,17 @@
         <f t="shared" si="0"/>
         <v>1895.6632653061224</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="5">
+        <v>2015</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="C14" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update treatment and AE cost tables
</commit_message>
<xml_diff>
--- a/data-raw/costs_ae.xlsx
+++ b/data-raw/costs_ae.xlsx
@@ -133,7 +133,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -570,7 +569,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -863,17 +862,17 @@
         <v>21</v>
       </c>
       <c r="C10" s="3">
-        <v>15709</v>
+        <v>940</v>
       </c>
       <c r="D10" s="1">
-        <v>11315</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1">
-        <v>21373</v>
+        <v>1844</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>2565.8163265306125</v>
+        <v>443.36734693877554</v>
       </c>
       <c r="G10" s="5">
         <v>2015</v>

</xml_diff>